<commit_message>
minor change to help and autosave
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>AUTOSAVE FIELDS</t>
   </si>
@@ -185,15 +185,6 @@
   </si>
   <si>
     <t>From Roast&gt;Properties&gt;Moisture Green</t>
-  </si>
-  <si>
-    <t>~moisturetunits</t>
-  </si>
-  <si>
-    <t>From Roast&gt;Properties&gt;Moisture</t>
-  </si>
-  <si>
-    <t>pct</t>
   </si>
   <si>
     <t>~machine</t>
@@ -1047,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1126,7 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -1146,7 +1137,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -1182,7 +1173,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1324,18 +1315,7 @@
       <c r="B25" t="s">
         <v>61</v>
       </c>
-      <c r="C25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26">
+      <c r="C25">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-updates inter-app operation on WIndows
-fix exception with background image entering designer mode
-update autosave help
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>AUTOSAVE FIELDS</t>
   </si>
@@ -209,6 +209,20 @@
   </si>
   <si>
     <t>The first 30 characters of the first line \nFrom Roast&gt;Properties&gt;Beans</t>
+  </si>
+  <si>
+    <t>bn:NOTES:
+Anything between single quotes ' will show in the file name only when ON.
+Example: 'REC ~batch'
+Anything between double quotes " will show in the file name only when OFF. 
+Example: "~operator"
+For backward compatibility, when the Prefix field is text only the date and time are appended to the file name.
+Example: 'Autosave' will result in file name 'Autosave_20-01-13_1705'.
+To show only the text place a single '!' at the start of the Prefix field
+Example: '!Autosave' will result in file name 'Autosave'.
+To maintain cross platform compatibility, file names may contain only letters, numbers, spaces, 
+and the following special characters:  
+_ - . ( )</t>
   </si>
 </sst>
 </file>
@@ -693,9 +707,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1038,11 +1055,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1319,6 +1334,11 @@
         <v>64</v>
       </c>
     </row>
+    <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-ignores case when matching autosave and eventsannotations fields
-corrected an issue in event annotation example 
-autosave match fields in one language
-update autosave help
-corrected issue identifying instance in comparator.py
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -229,7 +229,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,6 +361,19 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -707,10 +720,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1057,7 +1071,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1082,260 +1098,260 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>64</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>1742</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B21" t="s">
         <v>51</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>756.4</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B22" t="s">
         <v>53</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>11.7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B24" t="s">
         <v>58</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B25" t="s">
         <v>61</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adds post roast fields to autosave file names
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Autosave" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="151">
   <si>
     <t>AUTOSAVE FIELDS</t>
   </si>
@@ -62,9 +62,6 @@
     <t>~batch_long</t>
   </si>
   <si>
-    <t>Same as Batch field in Roast Properties\n "~batchprefix~batchnum (~batchposition)"</t>
-  </si>
-  <si>
     <t>Prod-653 (9)</t>
   </si>
   <si>
@@ -74,12 +71,6 @@
     <t>Ethiopia Guji</t>
   </si>
   <si>
-    <t>~beans</t>
-  </si>
-  <si>
-    <t>Ethiopia Guji purchased from R</t>
-  </si>
-  <si>
     <t>~beans_line</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
   </si>
   <si>
     <t>From Roast&gt;Properties&gt;Title</t>
-  </si>
-  <si>
-    <t>The first 30 characters of the first line \nFrom Roast&gt;Properties&gt;Beans</t>
   </si>
   <si>
     <t>bn:NOTES:
@@ -263,6 +251,241 @@
   </si>
   <si>
     <t>Burundi Roasted on 20-04-25.alog</t>
+  </si>
+  <si>
+    <t>~beans_nn</t>
+  </si>
+  <si>
+    <t>Ethiopia G</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Weight Roasted</t>
+  </si>
+  <si>
+    <t>~roastweight</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Volume Roasted</t>
+  </si>
+  <si>
+    <t>~roastvolume</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Density Roasted</t>
+  </si>
+  <si>
+    <t>~roastdensity</t>
+  </si>
+  <si>
+    <t>~roastmoisture</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Moisture Roasted</t>
+  </si>
+  <si>
+    <t>~colorwhole</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Color Whole</t>
+  </si>
+  <si>
+    <t>~colorground</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Color Ground</t>
+  </si>
+  <si>
+    <t>~colorsystem</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Color System</t>
+  </si>
+  <si>
+    <t>Tonino</t>
+  </si>
+  <si>
+    <t>~screenmin</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Screen Min</t>
+  </si>
+  <si>
+    <t>~screenmax</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Screen Max</t>
+  </si>
+  <si>
+    <t>~greenstemp</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;(Green) Beans Temperature</t>
+  </si>
+  <si>
+    <t>~ambtemp</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Ambient Temperature</t>
+  </si>
+  <si>
+    <t>~ambhumidity</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Ambient Humidity</t>
+  </si>
+  <si>
+    <t>~ambpressure</t>
+  </si>
+  <si>
+    <t>From Roast&gt;Properties&gt;Ambient Pressure</t>
+  </si>
+  <si>
+    <t>~auc</t>
+  </si>
+  <si>
+    <t>From the Profile Statistics - AUC</t>
+  </si>
+  <si>
+    <t>~aucbase</t>
+  </si>
+  <si>
+    <t>From the Profile Statistics - AUC Base</t>
+  </si>
+  <si>
+    <t>~chargeet</t>
+  </si>
+  <si>
+    <t>From the Profile - ET at CHARGE</t>
+  </si>
+  <si>
+    <t>~chargebt</t>
+  </si>
+  <si>
+    <t>From the Profile - BT at CHARGE</t>
+  </si>
+  <si>
+    <t>~fcset</t>
+  </si>
+  <si>
+    <t>From the Profile - ET at FCs</t>
+  </si>
+  <si>
+    <t>~fcsbt</t>
+  </si>
+  <si>
+    <t>From the Profile -BT at FCs</t>
+  </si>
+  <si>
+    <t>~dropet</t>
+  </si>
+  <si>
+    <t>From the Profile - ET at DROP</t>
+  </si>
+  <si>
+    <t>~dropbt</t>
+  </si>
+  <si>
+    <t>From the Profile - BT at DROP</t>
+  </si>
+  <si>
+    <t>~droptime</t>
+  </si>
+  <si>
+    <t>From the Profile - DROP time in seconds</t>
+  </si>
+  <si>
+    <t>617.0</t>
+  </si>
+  <si>
+    <t>Same as Batch field in Roast Properties
+"~batchprefix~batchnum (~batchposition)"</t>
+  </si>
+  <si>
+    <t>Replace “nn” with 10, 15, 20, 25, or 30 to show the first “nn” characters of the Beans field.
+From Roast&gt;Properties&gt;Beans</t>
+  </si>
+  <si>
+    <t>68.0</t>
+  </si>
+  <si>
+    <t>70.0</t>
+  </si>
+  <si>
+    <t>~droptime_long</t>
+  </si>
+  <si>
+    <t>From the Profile - DROP time in min_secs</t>
+  </si>
+  <si>
+    <t>10_17</t>
+  </si>
+  <si>
+    <t>~dtr</t>
+  </si>
+  <si>
+    <t>From Profile Statistics - DTR (in percent)</t>
+  </si>
+  <si>
+    <t>~roastingnotes_nn</t>
+  </si>
+  <si>
+    <t>~roastingnotes_line</t>
+  </si>
+  <si>
+    <t>Replace “nn” with 10, 15, 20, 25, or 30 to show the first “nn” characters of the Roasting Notes field.
+From Roast&gt;Properties&gt;Roasting Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No crash, </t>
+  </si>
+  <si>
+    <t>No crash, maintained RoR</t>
+  </si>
+  <si>
+    <t>Replace “nn” with 10, 15, 20, 25, or 30 to show the first “nn” characters of the Cupping Notes field.
+From Roast&gt;Properties&gt;Cupping Notes</t>
+  </si>
+  <si>
+    <t>The entire first line From Roast&gt;Properties&gt;Cupping Notes</t>
+  </si>
+  <si>
+    <t>The entire first line From Roast&gt;Properties&gt;Roasting Notes</t>
+  </si>
+  <si>
+    <t>Lots of berries and chocolate</t>
+  </si>
+  <si>
+    <t>Lots of be</t>
+  </si>
+  <si>
+    <t>~weightloss</t>
+  </si>
+  <si>
+    <t>~densityloss</t>
+  </si>
+  <si>
+    <t>~volumegain</t>
+  </si>
+  <si>
+    <t>Calculated volume gain in percent</t>
+  </si>
+  <si>
+    <t>Calculated weight loss in percent (the  “-” sign is not shown, it can be added manually in front of the field if desired)</t>
+  </si>
+  <si>
+    <t>Calculated density loss in percent (the  “-” sign is not shown, it can be added manually in front of the field if desired)</t>
+  </si>
+  <si>
+    <t>~moistureloss</t>
+  </si>
+  <si>
+    <t>Calculated moisture loss in percent (the  “-” sign is not shown, it can be added manually in front of the field if desired)</t>
+  </si>
+  <si>
+    <t>~cupptingnotes_nn</t>
+  </si>
+  <si>
+    <t>~cupptingnotes_line</t>
   </si>
 </sst>
 </file>
@@ -760,17 +983,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1113,16 +1336,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="76.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,78 +1409,78 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>64</v>
+        <v>74</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1">
         <v>1742</v>
@@ -1264,43 +1488,43 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1308,95 +1532,521 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.6</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="1">
-        <v>4.0999999999999996</v>
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>145</v>
+      </c>
+      <c r="C20" s="1">
+        <v>14.1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1">
-        <v>756.4</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
+      </c>
+      <c r="C22" s="1">
+        <v>6.8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="1">
-        <v>11.7</v>
+        <v>45</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>143</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>59</v>
+        <v>144</v>
+      </c>
+      <c r="C24" s="1">
+        <v>61.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1">
+        <v>756.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="1">
+        <v>375.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="1">
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="1">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="1">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="1">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1023.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="1">
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" s="1">
+        <v>379.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="1">
+        <v>375.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="1">
+        <v>397.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="1">
+        <v>386.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" s="1">
+        <v>378.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="1">
+        <v>412.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>65</v>
+      <c r="C58" s="5"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="C63" s="5"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="C64" s="5"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="C65" s="5"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="C66" s="5"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="C67" s="5"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="C68" s="5"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="C69" s="5"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="C70" s="5"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="C71" s="5"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="C72" s="5"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="C73" s="5"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="C74" s="5"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="C75" s="5"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +2058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1418,52 +2068,52 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>72</v>
+      <c r="B7" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-adds additional date and time fields to autosave
-fixed special event annotations will show when there is no DROP event
-fixed enable for individual special event annotation in the background
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
   <si>
     <t>AUTOSAVE FIELDS</t>
   </si>
@@ -507,6 +507,66 @@
   </si>
   <si>
     <t>~roastedmoisture</t>
+  </si>
+  <si>
+    <t>~yyyy</t>
+  </si>
+  <si>
+    <t>Roast year in format yyyy</t>
+  </si>
+  <si>
+    <t>~yy</t>
+  </si>
+  <si>
+    <t>Roast year in format yy</t>
+  </si>
+  <si>
+    <t>~mmm</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Roast month in format MM</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>~mm</t>
+  </si>
+  <si>
+    <t>~ddd</t>
+  </si>
+  <si>
+    <t>Roast month in format MMM (localized)</t>
+  </si>
+  <si>
+    <t>Roast day in format ddd (localized)</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Roast day in format dd</t>
+  </si>
+  <si>
+    <t>~dd</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>~hour</t>
+  </si>
+  <si>
+    <t>~minute</t>
+  </si>
+  <si>
+    <t>Roast hour in format hh</t>
+  </si>
+  <si>
+    <t>Roast minute in format mm</t>
   </si>
 </sst>
 </file>
@@ -1358,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,535 +1592,591 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>159</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2020</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>152</v>
+        <v>161</v>
+      </c>
+      <c r="C17" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>37</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3</v>
+        <v>164</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2.6</v>
+        <v>169</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>41</v>
+        <v>171</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="C22" s="1">
-        <v>14.1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="1">
         <v>42</v>
-      </c>
-      <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="1">
-        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="1">
-        <v>6.8</v>
+        <v>35</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="1">
-        <v>61.5</v>
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1">
-        <v>756.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C28" s="1">
-        <v>375.2</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" s="1">
-        <v>46.8</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1">
-        <v>11.7</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1">
-        <v>2.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>142</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C33" s="1">
-        <v>8.1</v>
+        <v>45</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="C34" s="1">
-        <v>64</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1">
-        <v>103</v>
+        <v>756.4</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C36" s="1">
-        <v>98</v>
+        <v>375.2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="C38" s="1">
-        <v>16</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1">
-        <v>18</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>157</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>119</v>
+        <v>79</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2.8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>120</v>
+        <v>143</v>
+      </c>
+      <c r="C41" s="1">
+        <v>8.1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="C42" s="1">
-        <v>35.1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C43" s="1">
-        <v>1023.8</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>146</v>
+        <v>82</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>83</v>
       </c>
       <c r="C44" s="1">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>147</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>150</v>
+        <v>85</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="C46" s="1">
-        <v>22.1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1">
-        <v>218</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="1">
-        <v>300</v>
+        <v>92</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="1">
-        <v>379.4</v>
+        <v>94</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C50" s="1">
-        <v>375.2</v>
+        <v>35.1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C51" s="1">
-        <v>397.4</v>
+        <v>1023.8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="C52" s="1">
-        <v>386.7</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="1">
-        <v>378.6</v>
+        <v>149</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1">
-        <v>412.5</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="5">
-        <v>617</v>
+        <v>100</v>
+      </c>
+      <c r="C55" s="1">
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="C56" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>129</v>
+        <v>103</v>
+      </c>
+      <c r="B57" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="1">
+        <v>379.4</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C58" s="1">
+        <v>375.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>135</v>
+        <v>107</v>
+      </c>
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="1">
+        <v>397.4</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="1">
+        <v>386.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="1">
+        <v>378.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="1">
+        <v>412.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="5">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B68" t="s">
         <v>132</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="C64" s="5"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="C66" s="5"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="C68" s="5"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
       <c r="C69" s="5"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2100,7 +2216,39 @@
       <c r="C78" s="5"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="1"/>
+      <c r="C79" s="5"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="C80" s="5"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="C81" s="5"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="C83" s="5"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="C84" s="5"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="C85" s="5"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="C86" s="5"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-adds a flag to place autosaved files on the recent file list
-adds current time to the autosave fields (~currtime)
-updates autosave help
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Autosave" sheetId="1" r:id="rId1"/>
-    <sheet name="Examples" sheetId="2" r:id="rId2"/>
+    <sheet name="Autosave" sheetId="3" r:id="rId1"/>
+    <sheet name="Autosave Fields" sheetId="1" r:id="rId2"/>
+    <sheet name="Examples" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="199">
   <si>
     <t>AUTOSAVE FIELDS</t>
   </si>
@@ -567,6 +568,75 @@
   </si>
   <si>
     <t>Roast minute in format mm</t>
+  </si>
+  <si>
+    <t>AUTOSAVE DIALOG</t>
+  </si>
+  <si>
+    <t>Autosave [a]</t>
+  </si>
+  <si>
+    <t>Add to recent file list</t>
+  </si>
+  <si>
+    <t>File Name Prefix</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>Save Also</t>
+  </si>
+  <si>
+    <t>When checked, Autosaved files will be added to the Files&gt;&gt; Open Recent files list.</t>
+  </si>
+  <si>
+    <t>Allows to save an additional file.  Choose the file type from the pull-down menu.</t>
+  </si>
+  <si>
+    <t>Where to store the Autosaved files.</t>
+  </si>
+  <si>
+    <t>Where to store the additional files.</t>
+  </si>
+  <si>
+    <t>Defines the file name to use for Autosave.  See the Autosave Fields section below.</t>
+  </si>
+  <si>
+    <t>Preview:</t>
+  </si>
+  <si>
+    <t>Shows an example of the file name based on the File Name Prefix field.
+A 'While Recording:' example will also be shown if the file name will be different when the scope is sampling.</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Dialog Field</t>
+  </si>
+  <si>
+    <t>Turn Autosave ON or OFF.  When sampling, the keyboard 'a' will save the profile at that moment.
+NOTE: Files with the same file name will be silently overwritten.  Use ~currdatetime in the file name prefix to get unique file names.</t>
+  </si>
+  <si>
+    <t>~currtime</t>
+  </si>
+  <si>
+    <t>21-01-18_093609</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current date and time with seconds in format yy-MM-dd_hhmmss.  Not the same as roast time. </t>
+  </si>
+  <si>
+    <t>\u0027Recording ~batchcounter' "~batch" ~title ~date_long_'~currtime'"~time"</t>
+  </si>
+  <si>
+    <t>Creates a unique filename for multiple saves while sampling by using ~currtime.
+When OFF:
+Prod-1380 Burundi Kiganda Murambi 2020-04-25_1136.alog
+While Recording. 
+Recording 1380  Burundi KigandaMurambi 2020-04-25_113809.alog</t>
   </si>
 </sst>
 </file>
@@ -1418,10 +1488,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="86.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C88"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,507 +1838,514 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>151</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>152</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3</v>
+        <v>55</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>154</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1">
-        <v>2.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>76</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2.6</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>136</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="1">
-        <v>14.1</v>
+        <v>40</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="C31" s="1">
-        <v>4.0999999999999996</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>155</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1">
-        <v>6.8</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>77</v>
+      </c>
+      <c r="C33" s="1">
+        <v>6.8</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34" s="1">
-        <v>61.5</v>
+        <v>45</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>139</v>
       </c>
       <c r="C35" s="1">
-        <v>756.4</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>156</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1">
-        <v>375.2</v>
+        <v>756.4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>49</v>
+        <v>156</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>51</v>
+        <v>78</v>
+      </c>
+      <c r="C37" s="1">
+        <v>375.2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>137</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>141</v>
-      </c>
-      <c r="C38" s="1">
-        <v>46.8</v>
+        <v>50</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="C39" s="1">
-        <v>11.7</v>
+        <v>46.8</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>157</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="C40" s="1">
-        <v>2.8</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
       <c r="C41" s="1">
-        <v>8.1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>143</v>
       </c>
       <c r="C42" s="1">
-        <v>64</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1">
-        <v>103</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" s="1">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
+      </c>
+      <c r="C45" s="1">
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="1">
-        <v>16</v>
+        <v>85</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="C48" s="1">
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="1">
-        <v>35.1</v>
+        <v>94</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C51" s="1">
-        <v>1023.8</v>
+        <v>35.1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="C52" s="1">
-        <v>112</v>
+        <v>1023.8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>149</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
+      </c>
+      <c r="C53" s="1">
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" s="1">
-        <v>22.1</v>
+        <v>149</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="B55" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C55" s="1">
-        <v>218</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C56" s="1">
-        <v>300</v>
+        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C57" s="1">
-        <v>379.4</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C58" s="1">
-        <v>375.2</v>
+        <v>379.4</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C59" s="1">
-        <v>397.4</v>
+        <v>375.2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C60" s="1">
-        <v>386.7</v>
+        <v>397.4</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C61" s="1">
-        <v>378.6</v>
+        <v>386.7</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C62" s="1">
-        <v>412.5</v>
+        <v>378.6</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B63" t="s">
-        <v>116</v>
-      </c>
-      <c r="C63" s="5">
-        <v>617</v>
+        <v>114</v>
+      </c>
+      <c r="C63" s="1">
+        <v>412.5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="5">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>122</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>132</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C69" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="5"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
       <c r="C70" s="5"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2248,20 +2413,24 @@
       <c r="C86" s="5"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="C87" s="5"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2319,6 +2488,14 @@
         <v>68</v>
       </c>
     </row>
+    <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- added burnerlabels to the Source strings so that the data table cells for Source are more meaningful
- finished adding BBP after preheat and removed roasts per session
    - plumbed aw.qmc.betweenbatch_after_preheat and aw.qmc.roastbatchpos into the energy calculation
    - removed all traces of aw.qmc.roasts_per_session and aw.qmc.roasts_per_session_setup from main.py
    - renamed updateBBBafterPreHeat() to updateBBPafterPreHeat()
    - added self.updateMetricsLabel() to updateBBPafterPreHeat()
- moved co2_per_green_kg calculation to calcEnergyuse() and per_roastedkg is completely removed.
- when green weight is zero use uuu rather than a blank field in MetricsLabel (for discussion)
- added calculated energy fields to autosave
- added calculated energy fields to Excel and CSV ranking reports
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Autosave" sheetId="3" r:id="rId1"/>
     <sheet name="Autosave Fields" sheetId="1" r:id="rId2"/>
     <sheet name="Examples" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="217">
   <si>
     <t>AUTOSAVE FIELDS</t>
   </si>
@@ -637,6 +637,60 @@
 Prod-1380 Burundi Kiganda Murambi 2020-04-25_1136.alog
 While Recording. 
 Recording 1380  Burundi KigandaMurambi 2020-04-25_113809.alog</t>
+  </si>
+  <si>
+    <t>~btubatch</t>
+  </si>
+  <si>
+    <t>~co2batch</t>
+  </si>
+  <si>
+    <t>~btupreheat</t>
+  </si>
+  <si>
+    <t>~co2preheat</t>
+  </si>
+  <si>
+    <t>~btubbp</t>
+  </si>
+  <si>
+    <t>~co2bbp</t>
+  </si>
+  <si>
+    <t>~bturoast</t>
+  </si>
+  <si>
+    <t>~co2roast</t>
+  </si>
+  <si>
+    <t>~co2pergreenkg</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - CO2 produced by the batch in g</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - Energy used during preheat in BTU</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - Total energy used by the batch in BTU</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - Energy used from CHARGE to DROP in BTU</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - Energy used during Between Batch Protocol in BTU</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - CO2 produced from CHARGE to DROP in g</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - CO2 produced during Between Batch Protocol in g</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - CO2 produced during preheat in g</t>
+  </si>
+  <si>
+    <t>From the Profile Energy Use - CO2 produced per kg of green beans in g</t>
   </si>
 </sst>
 </file>
@@ -1576,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,45 +2397,108 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C70" s="5">
+        <v>8943.2000000000007</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" s="5">
+        <v>923.3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" s="5">
+        <v>2538.8000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C73" s="5">
+        <v>443.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C74" s="5">
+        <v>1019.7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C75" s="5">
+        <v>254.1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C76" s="5">
+        <v>7843.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C77" s="5">
+        <v>873.9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C78" s="5">
+        <v>354.3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C70" s="5"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="C71" s="5"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="C72" s="5"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="C73" s="5"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="C74" s="5"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="C77" s="5"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
       <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -2417,7 +2534,43 @@
       <c r="C87" s="5"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
+      <c r="A88" s="1"/>
+      <c r="C88" s="5"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="C89" s="5"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="C90" s="5"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="C91" s="5"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="C92" s="5"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="C93" s="5"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="C94" s="5"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="C95" s="5"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="C96" s="5"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2428,7 +2581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
-add fields to autosave
-autosave respect decimal places setting where applicable
- enhance type hints
-fix typo
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/autosave.xlsx
+++ b/doc/help_dialogs/Input_files/autosave.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roast\Documents\GitHub\artisan-roaster-scope\doc\help_dialogs\Input_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F054E15-F3AE-46CC-8DD2-C45A66D585BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Autosave" sheetId="3" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
   <si>
     <t>AUTOSAVE FIELDS</t>
   </si>
@@ -468,12 +474,6 @@
     <t>Calculated moisture loss in percent (the  “-” sign is not shown, it can be added manually in front of the field if desired)</t>
   </si>
   <si>
-    <t>~cupptingnotes_nn</t>
-  </si>
-  <si>
-    <t>~cupptingnotes_line</t>
-  </si>
-  <si>
     <t>~devtime</t>
   </si>
   <si>
@@ -692,11 +692,65 @@
   <si>
     <t>From the Profile Energy Use - CO2 produced per kg of green beans in g</t>
   </si>
+  <si>
+    <t>~fcstime</t>
+  </si>
+  <si>
+    <t>~fcstime_long</t>
+  </si>
+  <si>
+    <t>From the Profile - FCs time in seconds</t>
+  </si>
+  <si>
+    <t>From the Profile - FCs time in min_secs</t>
+  </si>
+  <si>
+    <t>08_10</t>
+  </si>
+  <si>
+    <t>~mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Config&gt;Temperature - the current temperature mode C or F.  </t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>~title ~weight~weightunits ~finishphase_deltatemp~mode</t>
+  </si>
+  <si>
+    <t>~cuppingnotes_nn</t>
+  </si>
+  <si>
+    <t>~cuppingnotes_line</t>
+  </si>
+  <si>
+    <t>~dryphasedeltatemp</t>
+  </si>
+  <si>
+    <t>~midphasedeltatemp</t>
+  </si>
+  <si>
+    <t>~finishphasedeltatemp</t>
+  </si>
+  <si>
+    <t>Burundi 454.0g 19.8F.alog</t>
+  </si>
+  <si>
+    <t>From the Profile - BT temperature change from TP to DRY</t>
+  </si>
+  <si>
+    <t>From the Profile - BT temperature change from DRY to FCs</t>
+  </si>
+  <si>
+    <t>From the Profile - BT temperature change from FCs to DROP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1188,7 +1242,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
@@ -1197,8 +1251,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1251,6 +1304,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1298,7 +1354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1331,9 +1387,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1366,6 +1439,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1541,86 +1631,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="86.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="86.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>179</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>180</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>181</v>
       </c>
-      <c r="B5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>183</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1629,26 +1719,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C97"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="76.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="76.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1659,7 +1749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1670,7 +1760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1681,7 +1771,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1692,7 +1782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1703,7 +1793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1714,7 +1804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1725,7 +1815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>74</v>
       </c>
@@ -1736,7 +1826,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1747,7 +1837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1758,7 +1848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1769,7 +1859,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -1780,7 +1870,7 @@
         <v>1742</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -1791,7 +1881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -1802,106 +1892,106 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C16" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C17" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B19" t="s">
         <v>162</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C19" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" t="s">
         <v>169</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B21" t="s">
-        <v>171</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B22" t="s">
         <v>174</v>
-      </c>
-      <c r="B22" t="s">
-        <v>176</v>
       </c>
       <c r="C22" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B23" t="s">
         <v>175</v>
-      </c>
-      <c r="B23" t="s">
-        <v>177</v>
       </c>
       <c r="C23" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" t="s">
         <v>194</v>
       </c>
-      <c r="B24" t="s">
-        <v>196</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1912,18 +2002,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" t="s">
         <v>151</v>
       </c>
-      <c r="B26" t="s">
-        <v>153</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
@@ -1934,7 +2024,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -1945,9 +2035,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B29" t="s">
         <v>76</v>
@@ -1956,7 +2046,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1967,7 +2057,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>136</v>
       </c>
@@ -1978,7 +2068,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1989,9 +2079,9 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B33" t="s">
         <v>77</v>
@@ -2000,7 +2090,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
@@ -2011,7 +2101,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>138</v>
       </c>
@@ -2022,7 +2112,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>47</v>
       </c>
@@ -2033,9 +2123,9 @@
         <v>756.4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B37" t="s">
         <v>78</v>
@@ -2044,7 +2134,7 @@
         <v>375.2</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>49</v>
       </c>
@@ -2055,7 +2145,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>137</v>
       </c>
@@ -2066,7 +2156,7 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -2077,9 +2167,9 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B41" t="s">
         <v>79</v>
@@ -2088,7 +2178,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>142</v>
       </c>
@@ -2099,7 +2189,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -2110,7 +2200,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>80</v>
       </c>
@@ -2121,7 +2211,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>82</v>
       </c>
@@ -2132,7 +2222,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>84</v>
       </c>
@@ -2143,7 +2233,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>87</v>
       </c>
@@ -2154,7 +2244,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
@@ -2165,7 +2255,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>91</v>
       </c>
@@ -2176,7 +2266,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>93</v>
       </c>
@@ -2187,7 +2277,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>95</v>
       </c>
@@ -2198,7 +2288,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>97</v>
       </c>
@@ -2209,29 +2299,29 @@
         <v>1023.8</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" t="s">
         <v>146</v>
-      </c>
-      <c r="B53" t="s">
-        <v>148</v>
       </c>
       <c r="C53" s="1">
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" t="s">
         <v>147</v>
       </c>
-      <c r="B54" t="s">
-        <v>149</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>124</v>
       </c>
@@ -2242,7 +2332,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>99</v>
       </c>
@@ -2253,7 +2343,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>101</v>
       </c>
@@ -2264,313 +2354,379 @@
         <v>300</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" t="s">
+        <v>221</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C59" s="1">
         <v>379.4</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C60" s="1">
         <v>375.2</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C61" s="1">
         <v>397.4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C62" s="1">
         <v>386.7</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" t="s">
+        <v>217</v>
+      </c>
+      <c r="C63" s="1">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B64" t="s">
+        <v>218</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C65" s="1">
         <v>378.6</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B66" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C66" s="1">
         <v>412.5</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B67" t="s">
         <v>116</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C67" s="5">
         <v>617</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" t="s">
         <v>122</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C68" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69" t="s">
+        <v>230</v>
+      </c>
+      <c r="C69" s="5">
+        <v>121.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B70" t="s">
+        <v>231</v>
+      </c>
+      <c r="C70" s="5">
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B71" t="s">
+        <v>232</v>
+      </c>
+      <c r="C71" s="5">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B73" t="s">
         <v>133</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B68" s="4" t="s">
+    <row r="74" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B69" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75" t="s">
         <v>132</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C75" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C76" s="5">
+        <v>8943.2000000000007</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" s="5">
+        <v>923.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B78" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C78" s="5">
+        <v>2538.8000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C79" s="5">
+        <v>443.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C70" s="5">
-        <v>8943.2000000000007</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C71" s="5">
-        <v>923.3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B72" s="4" t="s">
+      <c r="C80" s="5">
+        <v>1019.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C81" s="5">
+        <v>254.1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C72" s="5">
-        <v>2538.8000000000002</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C73" s="5">
-        <v>443.9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C74" s="5">
-        <v>1019.7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="C82" s="5">
+        <v>7843.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B83" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C83" s="5">
+        <v>873.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B84" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C75" s="5">
-        <v>254.1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C76" s="5">
-        <v>7843.2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C77" s="5">
-        <v>873.9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="C78" s="5">
+      <c r="C84" s="5">
         <v>354.3</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="C81" s="5"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1"/>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1"/>
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="6"/>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+      <c r="C97" s="5"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+      <c r="C98" s="5"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+      <c r="C99" s="5"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+      <c r="C100" s="5"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+      <c r="C101" s="5"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+      <c r="C102" s="5"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2578,30 +2734,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" customWidth="1"/>
+    <col min="1" max="1" width="49.88671875" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -2609,7 +2765,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -2617,7 +2773,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -2625,7 +2781,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -2633,20 +2789,28 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B7" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>198</v>
+    <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>